<commit_message>
committing the main 5 repos source code + their results
</commit_message>
<xml_diff>
--- a/scalpel/typeinfer/evaluation/evaluation_outputs/beurtschipper__Depix.xlsx
+++ b/scalpel/typeinfer/evaluation/evaluation_outputs/beurtschipper__Depix.xlsx
@@ -618,7 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{'float', 'any', 'int'}</t>
+          <t>{'any', 'int', 'float'}</t>
         </is>
       </c>
     </row>
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1973,7 +1973,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>84.48</v>
+        <v>31.82</v>
       </c>
       <c r="E58" t="inlineStr"/>
     </row>

</xml_diff>